<commit_message>
Update package with all changes: themes, templates, and fixes
</commit_message>
<xml_diff>
--- a/data/lexemes.xlsx
+++ b/data/lexemes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergeimalyshev/Desktop/Tocharian/Tocharian A/My grammar/NewToch/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergeimalyshev/Desktop/Tocharian/Tocharian A/My grammar/Candrakanta/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCAC149-BAEE-2544-8929-9CEE536D7D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18144A1-09CE-9E48-9434-A77BB258CCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="1440" windowWidth="25700" windowHeight="13080" xr2:uid="{DFFD3512-190B-6C44-A03E-FE8C03207A6B}"/>
+    <workbookView xWindow="2220" yWindow="760" windowWidth="25700" windowHeight="13080" xr2:uid="{DFFD3512-190B-6C44-A03E-FE8C03207A6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Affixation" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="748">
   <si>
     <t>Shape</t>
   </si>
@@ -1157,12 +1157,6 @@
     <t>V_ṣtār</t>
   </si>
   <si>
-    <t>I_särki</t>
-  </si>
-  <si>
-    <t>behind</t>
-  </si>
-  <si>
     <t>R_sùkātik</t>
   </si>
   <si>
@@ -1328,9 +1322,6 @@
     <t>pause</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>W_zeke</t>
   </si>
   <si>
@@ -1610,9 +1601,6 @@
     <t>V_säl</t>
   </si>
   <si>
-    <t>M_särka</t>
-  </si>
-  <si>
     <t>PREF</t>
   </si>
   <si>
@@ -1706,12 +1694,6 @@
     <t>V_säqă</t>
   </si>
   <si>
-    <t>be.happy</t>
-  </si>
-  <si>
-    <t>be.glad</t>
-  </si>
-  <si>
     <t>V_klop</t>
   </si>
   <si>
@@ -1775,9 +1757,6 @@
     <t>I_lokeṃ</t>
   </si>
   <si>
-    <t>long.ago</t>
-  </si>
-  <si>
     <t>I_kāzekeṃ</t>
   </si>
   <si>
@@ -1787,9 +1766,6 @@
     <t>I_kāze</t>
   </si>
   <si>
-    <t>each.other</t>
-  </si>
-  <si>
     <t>X_ālamwäc</t>
   </si>
   <si>
@@ -1838,12 +1814,6 @@
     <t>I_kāmăr</t>
   </si>
   <si>
-    <t>full.sister</t>
-  </si>
-  <si>
-    <t>full.brother</t>
-  </si>
-  <si>
     <t>C_pracăr</t>
   </si>
   <si>
@@ -2277,6 +2247,39 @@
   </si>
   <si>
     <t>C_śriñkät</t>
+  </si>
+  <si>
+    <t>Kāsäwă</t>
+  </si>
+  <si>
+    <t>Riṣak;Kāsäwă</t>
+  </si>
+  <si>
+    <t>full brother</t>
+  </si>
+  <si>
+    <t>full sister</t>
+  </si>
+  <si>
+    <t>long ago</t>
+  </si>
+  <si>
+    <t>each other</t>
+  </si>
+  <si>
+    <t>be happy</t>
+  </si>
+  <si>
+    <t>be glad</t>
+  </si>
+  <si>
+    <t>Ṣomă</t>
+  </si>
+  <si>
+    <t>Morpheme_1</t>
+  </si>
+  <si>
+    <t>Morpheme_2</t>
   </si>
 </sst>
 </file>
@@ -2686,10 +2689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF76C2B-797E-2544-85E2-CF60CE11F59B}">
-  <dimension ref="A1:G265"/>
+  <dimension ref="A1:G264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="175" workbookViewId="0">
-      <selection activeCell="D200" sqref="D200"/>
+    <sheetView tabSelected="1" topLeftCell="A251" zoomScale="175" workbookViewId="0">
+      <selection activeCell="A264" sqref="A264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2710,30 +2713,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>430</v>
+        <v>746</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>430</v>
+        <v>747</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>430</v>
+        <v>747</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>724</v>
+        <v>714</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="D2" s="3">
         <v>3</v>
@@ -2761,24 +2764,24 @@
         <v>302</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>67</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>619</v>
+        <v>609</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>620</v>
+        <v>610</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>67</v>
@@ -2789,13 +2792,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>646</v>
+        <v>636</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>644</v>
+        <v>634</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>67</v>
@@ -2806,10 +2809,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>139</v>
@@ -2818,15 +2821,15 @@
         <v>67</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>224</v>
@@ -2857,7 +2860,7 @@
         <v>344</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>67</v>
@@ -2880,18 +2883,18 @@
         <v>67</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>623</v>
+        <v>613</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>67</v>
@@ -2902,13 +2905,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>67</v>
@@ -2928,7 +2931,7 @@
         <v>67</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -2961,30 +2964,30 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>742</v>
+        <v>732</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>743</v>
+        <v>733</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>744</v>
+        <v>734</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>67</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>615</v>
+        <v>605</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>642</v>
+        <v>632</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>67</v>
@@ -2995,13 +2998,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>67</v>
@@ -3009,13 +3012,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>389</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>67</v>
@@ -3023,13 +3026,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>638</v>
+        <v>628</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>639</v>
+        <v>629</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>67</v>
@@ -3040,33 +3043,33 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>571</v>
+        <v>738</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>617</v>
+        <v>607</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>618</v>
+        <v>608</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>3</v>
@@ -3080,7 +3083,7 @@
         <v>213</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>730</v>
+        <v>720</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>169</v>
@@ -3088,13 +3091,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>746</v>
+        <v>736</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>728</v>
+        <v>718</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>729</v>
+        <v>719</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>169</v>
@@ -3116,16 +3119,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>603</v>
+        <v>593</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>601</v>
+        <v>739</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>108</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>602</v>
+        <v>592</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -3133,7 +3136,7 @@
         <v>107</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>600</v>
+        <v>740</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>108</v>
@@ -3150,7 +3153,7 @@
         <v>187</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>189</v>
@@ -3173,7 +3176,7 @@
         <v>189</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -3184,10 +3187,10 @@
         <v>58</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>59</v>
@@ -3201,7 +3204,7 @@
         <v>95</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>37</v>
@@ -3223,7 +3226,7 @@
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="1" t="s">
-        <v>725</v>
+        <v>715</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -3258,10 +3261,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>75</v>
@@ -3273,7 +3276,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>699</v>
+        <v>689</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>15</v>
@@ -3290,7 +3293,7 @@
         <v>297</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>298</v>
@@ -3329,21 +3332,21 @@
         <v>82</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>720</v>
+        <v>710</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>628</v>
+        <v>618</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>629</v>
+        <v>619</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>630</v>
+        <v>620</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>82</v>
@@ -3357,24 +3360,24 @@
         <v>168</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>82</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>677</v>
+        <v>667</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>678</v>
+        <v>668</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>166</v>
@@ -3383,7 +3386,7 @@
         <v>82</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -3400,15 +3403,15 @@
         <v>82</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>741</v>
+        <v>731</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>12</v>
@@ -3423,16 +3426,16 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>737</v>
+        <v>727</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>738</v>
+        <v>728</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>739</v>
+        <v>729</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>740</v>
+        <v>730</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -3449,18 +3452,18 @@
         <v>47</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>47</v>
@@ -3488,13 +3491,13 @@
         <v>326</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -3514,13 +3517,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>47</v>
@@ -3528,13 +3531,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>671</v>
+        <v>661</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>672</v>
+        <v>662</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>47</v>
@@ -3582,7 +3585,7 @@
         <v>47</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -3599,18 +3602,18 @@
         <v>47</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>654</v>
+        <v>644</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>655</v>
+        <v>645</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>656</v>
+        <v>646</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>47</v>
@@ -3630,12 +3633,12 @@
         <v>47</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>170</v>
@@ -3647,15 +3650,15 @@
         <v>47</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>150</v>
@@ -3678,21 +3681,21 @@
         <v>47</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>47</v>
@@ -3700,30 +3703,30 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>156</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>47</v>
@@ -3743,18 +3746,18 @@
         <v>47</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>685</v>
+        <v>675</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>686</v>
+        <v>676</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>687</v>
+        <v>677</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>47</v>
@@ -3777,7 +3780,7 @@
         <v>47</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -3794,7 +3797,7 @@
         <v>47</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -3811,7 +3814,7 @@
         <v>47</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -3828,7 +3831,7 @@
         <v>47</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>722</v>
+        <v>712</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -3845,7 +3848,7 @@
         <v>47</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -3862,10 +3865,10 @@
         <v>47</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>681</v>
+        <v>671</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -3896,18 +3899,18 @@
         <v>47</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>424</v>
-      </c>
       <c r="C76" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>47</v>
@@ -3915,13 +3918,13 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>47</v>
@@ -3941,7 +3944,7 @@
         <v>47</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -3958,7 +3961,7 @@
         <v>47</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -3989,7 +3992,7 @@
         <v>47</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -4011,13 +4014,13 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>657</v>
+        <v>647</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>658</v>
+        <v>648</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>47</v>
@@ -4025,7 +4028,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>74</v>
@@ -4037,7 +4040,7 @@
         <v>47</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -4054,18 +4057,18 @@
         <v>47</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>47</v>
@@ -4087,30 +4090,30 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>191</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>47</v>
@@ -4130,18 +4133,18 @@
         <v>47</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>47</v>
@@ -4161,18 +4164,18 @@
         <v>47</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>180</v>
@@ -4183,13 +4186,13 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>47</v>
@@ -4203,7 +4206,7 @@
         <v>19</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>47</v>
@@ -4212,7 +4215,7 @@
         <v>2</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
@@ -4223,13 +4226,13 @@
         <v>346</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -4240,7 +4243,7 @@
         <v>310</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>47</v>
@@ -4248,27 +4251,27 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>710</v>
+        <v>700</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>342</v>
@@ -4291,7 +4294,7 @@
         <v>47</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -4325,7 +4328,7 @@
         <v>47</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
@@ -4347,13 +4350,13 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>47</v>
@@ -4361,13 +4364,13 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>47</v>
@@ -4375,22 +4378,22 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B106" s="1" t="s">
-        <v>386</v>
-      </c>
       <c r="C106" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>717</v>
+        <v>707</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
@@ -4423,13 +4426,13 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>627</v>
+        <v>617</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>126</v>
@@ -4437,7 +4440,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>50</v>
@@ -4457,7 +4460,7 @@
         <v>50</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>161</v>
@@ -4477,18 +4480,18 @@
         <v>161</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>161</v>
@@ -4511,44 +4514,44 @@
         <v>2</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>652</v>
+        <v>642</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>161</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>631</v>
+        <v>621</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>632</v>
+        <v>622</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>634</v>
+        <v>624</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>112</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>633</v>
+        <v>623</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
@@ -4565,7 +4568,7 @@
         <v>112</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>721</v>
+        <v>711</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
@@ -4590,7 +4593,7 @@
         <v>8</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>112</v>
@@ -4601,13 +4604,13 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>112</v>
@@ -4618,10 +4621,10 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>317</v>
@@ -4646,13 +4649,13 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>112</v>
@@ -4674,7 +4677,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>604</v>
+        <v>594</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>113</v>
@@ -4686,24 +4689,24 @@
         <v>112</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>112</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
@@ -4725,13 +4728,13 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>112</v>
@@ -4754,18 +4757,18 @@
         <v>3</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>112</v>
@@ -4773,7 +4776,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>229</v>
@@ -4785,7 +4788,7 @@
         <v>112</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>615</v>
+        <v>605</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
@@ -4832,47 +4835,47 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>191</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>112</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>392</v>
-      </c>
       <c r="C136" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>112</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D137" s="5" t="s">
         <v>112</v>
@@ -4880,13 +4883,13 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>745</v>
+        <v>735</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D138" s="5" t="s">
         <v>112</v>
@@ -4894,13 +4897,13 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>112</v>
@@ -4908,13 +4911,13 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>635</v>
+        <v>625</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>636</v>
+        <v>626</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>637</v>
+        <v>627</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>112</v>
@@ -4922,13 +4925,13 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>682</v>
+        <v>672</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>683</v>
+        <v>673</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>684</v>
+        <v>674</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>59</v>
@@ -4936,13 +4939,13 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>59</v>
@@ -4950,13 +4953,13 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>579</v>
+        <v>741</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>59</v>
@@ -4964,44 +4967,44 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>373</v>
+        <v>614</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>524</v>
+        <v>364</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="G144" s="1" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>624</v>
+        <v>601</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>365</v>
+        <v>602</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>364</v>
+        <v>603</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G145" s="1" t="s">
-        <v>571</v>
-      </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>611</v>
+        <v>655</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>612</v>
+        <v>657</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>613</v>
+        <v>656</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>59</v>
@@ -5009,13 +5012,13 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>665</v>
+        <v>530</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>667</v>
+        <v>532</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>666</v>
+        <v>441</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>59</v>
@@ -5023,13 +5026,13 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>534</v>
+        <v>341</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>444</v>
+        <v>342</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>59</v>
@@ -5037,75 +5040,75 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>341</v>
+        <v>264</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>535</v>
+        <v>110</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>342</v>
+        <v>265</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="G149" s="1" t="s">
+        <v>723</v>
+      </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>264</v>
+        <v>658</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>110</v>
+        <v>657</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>265</v>
+        <v>656</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G150" s="1" t="s">
-        <v>733</v>
+        <v>659</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>668</v>
+        <v>368</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>667</v>
+        <v>175</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>666</v>
+        <v>174</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>669</v>
+        <v>188</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>368</v>
+        <v>322</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>175</v>
+        <v>324</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>174</v>
+        <v>323</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F152" s="1" t="s">
-        <v>590</v>
-      </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>322</v>
+        <v>271</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>324</v>
+        <v>12</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>323</v>
+        <v>269</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>188</v>
@@ -5113,44 +5116,44 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>271</v>
+        <v>576</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>12</v>
+        <v>742</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>269</v>
+        <v>62</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>188</v>
+        <v>547</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>584</v>
+        <v>303</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>583</v>
+        <v>304</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>62</v>
+        <v>305</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>63</v>
+        <v>132</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>304</v>
+        <v>7</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>132</v>
@@ -5158,46 +5161,49 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>311</v>
+        <v>578</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>7</v>
+        <v>267</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>312</v>
+        <v>266</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>132</v>
       </c>
+      <c r="G157" s="1" t="s">
+        <v>604</v>
+      </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>586</v>
+        <v>417</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>267</v>
+        <v>418</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="D158" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D158" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="G158" s="1" t="s">
-        <v>614</v>
+      <c r="E158" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>419</v>
+        <v>211</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>420</v>
+        <v>212</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="D159" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D159" s="1" t="s">
         <v>132</v>
       </c>
       <c r="E159" s="1" t="s">
@@ -5206,13 +5212,13 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>211</v>
+        <v>416</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>212</v>
+        <v>419</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>56</v>
+        <v>414</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>132</v>
@@ -5223,148 +5229,145 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>418</v>
+        <v>52</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>421</v>
+        <v>53</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>416</v>
+        <v>51</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>98</v>
+        <v>521</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>52</v>
+        <v>277</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>53</v>
+        <v>278</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>51</v>
+        <v>538</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>525</v>
+        <v>521</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>721</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>277</v>
+        <v>693</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>278</v>
+        <v>695</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>542</v>
+        <v>694</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>731</v>
+        <v>562</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>703</v>
+        <v>272</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>705</v>
+        <v>273</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>704</v>
+        <v>142</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="G164" s="1" t="s">
-        <v>568</v>
+        <v>521</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>272</v>
+        <v>91</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>273</v>
+        <v>92</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>142</v>
+        <v>93</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>91</v>
+        <v>522</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>526</v>
+        <v>284</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>90</v>
+        <v>285</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>89</v>
+        <v>286</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>284</v>
+        <v>535</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>285</v>
+        <v>21</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>286</v>
+        <v>579</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>539</v>
+        <v>406</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>21</v>
+        <v>407</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>587</v>
+        <v>408</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>525</v>
+        <v>25</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>408</v>
+        <v>42</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>409</v>
+        <v>43</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>410</v>
+        <v>44</v>
       </c>
       <c r="D170" s="1" t="s">
         <v>25</v>
@@ -5372,13 +5375,13 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>42</v>
+        <v>404</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>43</v>
+        <v>405</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>44</v>
+        <v>139</v>
       </c>
       <c r="D171" s="1" t="s">
         <v>25</v>
@@ -5386,13 +5389,13 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>139</v>
+        <v>403</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>25</v>
@@ -5400,13 +5403,13 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>403</v>
+        <v>54</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>404</v>
+        <v>55</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>405</v>
+        <v>56</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>25</v>
@@ -5414,13 +5417,13 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>25</v>
@@ -5428,13 +5431,13 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D175" s="1" t="s">
         <v>25</v>
@@ -5442,237 +5445,240 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>20</v>
+        <v>716</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>23</v>
+        <v>529</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>726</v>
+        <v>611</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>533</v>
+        <v>612</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>6</v>
+        <v>523</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>621</v>
+        <v>686</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>622</v>
+        <v>687</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>527</v>
+        <v>688</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>696</v>
+        <v>488</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>697</v>
+        <v>490</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>698</v>
+        <v>489</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>491</v>
+        <v>162</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>493</v>
+        <v>48</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="D181" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D181" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>162</v>
+        <v>501</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>48</v>
+        <v>300</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D182" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="D182" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G182" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>504</v>
+        <v>200</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>300</v>
+        <v>202</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>616</v>
+        <v>201</v>
       </c>
       <c r="D183" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>200</v>
+        <v>38</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>202</v>
+        <v>39</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>201</v>
+        <v>40</v>
       </c>
       <c r="D184" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>76</v>
+        <v>669</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>77</v>
+        <v>670</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>679</v>
+        <v>280</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>680</v>
+        <v>281</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>73</v>
+        <v>282</v>
       </c>
       <c r="D187" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>280</v>
+        <v>708</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>281</v>
+        <v>499</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>282</v>
+        <v>709</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>718</v>
+        <v>157</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>502</v>
+        <v>156</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>719</v>
+        <v>553</v>
       </c>
       <c r="D189" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>157</v>
+        <v>681</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>156</v>
+        <v>682</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>559</v>
+        <v>197</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>691</v>
+        <v>219</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>692</v>
+        <v>221</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="D191" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>221</v>
+        <v>117</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>220</v>
+        <v>61</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>41</v>
@@ -5680,13 +5686,13 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>208</v>
+        <v>663</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>117</v>
+        <v>379</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>61</v>
+        <v>374</v>
       </c>
       <c r="D193" s="1" t="s">
         <v>41</v>
@@ -5694,13 +5700,13 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>673</v>
+        <v>558</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>381</v>
+        <v>65</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="D194" s="1" t="s">
         <v>41</v>
@@ -5708,13 +5714,13 @@
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>564</v>
+        <v>393</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>65</v>
+        <v>394</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>360</v>
+        <v>391</v>
       </c>
       <c r="D195" s="1" t="s">
         <v>41</v>
@@ -5722,13 +5728,13 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>395</v>
+        <v>182</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>396</v>
+        <v>181</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>393</v>
+        <v>183</v>
       </c>
       <c r="D196" s="1" t="s">
         <v>41</v>
@@ -5736,27 +5742,27 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>41</v>
+        <v>154</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>152</v>
+        <v>84</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>155</v>
+        <v>85</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>153</v>
+        <v>83</v>
       </c>
       <c r="D198" s="1" t="s">
         <v>154</v>
@@ -5764,44 +5770,44 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>84</v>
+        <v>496</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>85</v>
+        <v>497</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>83</v>
+        <v>498</v>
       </c>
       <c r="D199" s="1" t="s">
         <v>154</v>
       </c>
+      <c r="G199" s="1" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>499</v>
+        <v>216</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>500</v>
+        <v>218</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>501</v>
+        <v>217</v>
       </c>
       <c r="D200" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G200" s="1" t="s">
-        <v>607</v>
-      </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>216</v>
+        <v>491</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>218</v>
+        <v>492</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="D201" s="1" t="s">
         <v>154</v>
@@ -5809,13 +5815,13 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>494</v>
+        <v>690</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>495</v>
+        <v>691</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D202" s="1" t="s">
         <v>154</v>
@@ -5823,13 +5829,13 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>701</v>
+        <v>499</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>228</v>
+        <v>500</v>
       </c>
       <c r="D203" s="1" t="s">
         <v>154</v>
@@ -5837,13 +5843,13 @@
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>702</v>
+        <v>493</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="D204" s="1" t="s">
         <v>154</v>
@@ -5851,13 +5857,13 @@
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>496</v>
+        <v>185</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>498</v>
+        <v>184</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>497</v>
+        <v>186</v>
       </c>
       <c r="D205" s="1" t="s">
         <v>154</v>
@@ -5865,13 +5871,13 @@
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>185</v>
+        <v>333</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>184</v>
+        <v>335</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>186</v>
+        <v>334</v>
       </c>
       <c r="D206" s="1" t="s">
         <v>154</v>
@@ -5879,13 +5885,13 @@
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>333</v>
+        <v>724</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>335</v>
+        <v>725</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>334</v>
+        <v>726</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>154</v>
@@ -5893,13 +5899,13 @@
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>734</v>
+        <v>328</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>735</v>
+        <v>329</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>736</v>
+        <v>325</v>
       </c>
       <c r="D208" s="1" t="s">
         <v>154</v>
@@ -5907,13 +5913,13 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>325</v>
+        <v>337</v>
       </c>
       <c r="D209" s="1" t="s">
         <v>154</v>
@@ -5921,13 +5927,13 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>338</v>
+        <v>49</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="D210" s="1" t="s">
         <v>154</v>
@@ -5935,13 +5941,13 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>339</v>
+        <v>706</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>49</v>
+        <v>705</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>340</v>
+        <v>704</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>154</v>
@@ -5949,27 +5955,27 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>716</v>
+        <v>589</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>715</v>
+        <v>590</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>714</v>
+        <v>591</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>597</v>
+        <v>179</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>598</v>
+        <v>178</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>599</v>
+        <v>177</v>
       </c>
       <c r="D213" s="1" t="s">
         <v>172</v>
@@ -5977,13 +5983,13 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>179</v>
+        <v>502</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>178</v>
+        <v>490</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>177</v>
+        <v>489</v>
       </c>
       <c r="D214" s="1" t="s">
         <v>172</v>
@@ -5991,13 +5997,13 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>505</v>
+        <v>680</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>493</v>
+        <v>679</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>492</v>
+        <v>678</v>
       </c>
       <c r="D215" s="1" t="s">
         <v>172</v>
@@ -6005,13 +6011,13 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>690</v>
+        <v>256</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>689</v>
+        <v>257</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>688</v>
+        <v>258</v>
       </c>
       <c r="D216" s="1" t="s">
         <v>172</v>
@@ -6019,13 +6025,13 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>256</v>
+        <v>664</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>257</v>
+        <v>665</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>258</v>
+        <v>666</v>
       </c>
       <c r="D217" s="1" t="s">
         <v>172</v>
@@ -6033,13 +6039,13 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>674</v>
+        <v>595</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>675</v>
+        <v>596</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>676</v>
+        <v>122</v>
       </c>
       <c r="D218" s="1" t="s">
         <v>172</v>
@@ -6047,13 +6053,13 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>605</v>
+        <v>561</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>606</v>
+        <v>171</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>122</v>
+        <v>559</v>
       </c>
       <c r="D219" s="1" t="s">
         <v>172</v>
@@ -6061,13 +6067,13 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>567</v>
+        <v>203</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>171</v>
+        <v>117</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>565</v>
+        <v>204</v>
       </c>
       <c r="D220" s="1" t="s">
         <v>172</v>
@@ -6075,279 +6081,282 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>203</v>
+        <v>599</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C221" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D221" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C221" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D221" s="4" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>609</v>
+        <v>600</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C222" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D222" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D222" s="1" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>610</v>
+        <v>70</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>338</v>
+        <v>60</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>337</v>
+        <v>6</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>172</v>
+        <v>5</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>70</v>
+        <v>196</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>60</v>
+        <v>584</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>6</v>
+        <v>195</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>196</v>
+        <v>370</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>592</v>
+        <v>369</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>195</v>
+        <v>533</v>
       </c>
       <c r="D225" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>370</v>
+        <v>151</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>369</v>
+        <v>149</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>537</v>
+        <v>150</v>
       </c>
       <c r="D226" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>151</v>
+        <v>503</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>149</v>
+        <v>492</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>150</v>
+        <v>231</v>
       </c>
       <c r="D227" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>495</v>
+        <v>505</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>231</v>
+        <v>421</v>
       </c>
       <c r="D228" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>507</v>
+        <v>375</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>508</v>
+        <v>376</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>423</v>
+        <v>174</v>
       </c>
       <c r="D229" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>377</v>
+        <v>506</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>378</v>
+        <v>507</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>174</v>
+        <v>548</v>
       </c>
       <c r="D230" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>509</v>
+        <v>585</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>510</v>
+        <v>586</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>552</v>
+        <v>587</v>
       </c>
       <c r="D231" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>593</v>
+        <v>5</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>594</v>
+        <v>22</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>595</v>
+        <v>4</v>
       </c>
       <c r="D232" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>5</v>
+        <v>355</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>22</v>
+        <v>356</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>4</v>
+        <v>524</v>
       </c>
       <c r="D233" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>355</v>
+        <v>512</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>356</v>
+        <v>514</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>528</v>
+        <v>513</v>
       </c>
       <c r="D234" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A235" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D235" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A235" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="B235" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="C235" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="D235" s="1" t="s">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A236" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D236" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A236" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B236" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C236" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D236" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
-        <v>363</v>
+        <v>250</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>365</v>
+        <v>251</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>364</v>
+        <v>252</v>
       </c>
       <c r="D237" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G237" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
-        <v>250</v>
+        <v>509</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>251</v>
+        <v>492</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="D238" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
-        <v>512</v>
+        <v>292</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>495</v>
+        <v>293</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>231</v>
+        <v>56</v>
       </c>
       <c r="D239" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>293</v>
+        <v>508</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>56</v>
+        <v>276</v>
       </c>
       <c r="D240" s="1" t="s">
         <v>115</v>
@@ -6355,13 +6364,13 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
-        <v>279</v>
+        <v>510</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>511</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="D241" s="1" t="s">
         <v>115</v>
@@ -6369,13 +6378,13 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
-        <v>513</v>
+        <v>114</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>514</v>
+        <v>117</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>269</v>
+        <v>116</v>
       </c>
       <c r="D242" s="1" t="s">
         <v>115</v>
@@ -6383,13 +6392,13 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
-        <v>114</v>
+        <v>640</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>117</v>
+        <v>641</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>116</v>
+        <v>353</v>
       </c>
       <c r="D243" s="1" t="s">
         <v>115</v>
@@ -6397,13 +6406,13 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
-        <v>650</v>
+        <v>347</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>651</v>
+        <v>348</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="D244" s="1" t="s">
         <v>115</v>
@@ -6411,13 +6420,13 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
-        <v>347</v>
+        <v>536</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>348</v>
+        <v>511</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>345</v>
+        <v>268</v>
       </c>
       <c r="D245" s="1" t="s">
         <v>115</v>
@@ -6425,27 +6434,27 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
-        <v>540</v>
+        <v>701</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>514</v>
+        <v>702</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>268</v>
+        <v>703</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>115</v>
+        <v>35</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
-        <v>711</v>
+        <v>131</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>712</v>
+        <v>130</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>713</v>
+        <v>129</v>
       </c>
       <c r="D247" s="1" t="s">
         <v>35</v>
@@ -6453,13 +6462,13 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D248" s="1" t="s">
         <v>35</v>
@@ -6467,13 +6476,13 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
-        <v>123</v>
+        <v>486</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>124</v>
+        <v>165</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="D249" s="1" t="s">
         <v>35</v>
@@ -6481,13 +6490,13 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
-        <v>489</v>
+        <v>515</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>165</v>
+        <v>516</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>135</v>
+        <v>517</v>
       </c>
       <c r="D250" s="1" t="s">
         <v>35</v>
@@ -6495,13 +6504,13 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
-        <v>518</v>
+        <v>487</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>519</v>
+        <v>394</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>520</v>
+        <v>28</v>
       </c>
       <c r="D251" s="1" t="s">
         <v>35</v>
@@ -6509,13 +6518,13 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
-        <v>490</v>
+        <v>518</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>396</v>
+        <v>519</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>28</v>
+        <v>520</v>
       </c>
       <c r="D252" s="1" t="s">
         <v>35</v>
@@ -6523,13 +6532,13 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
-        <v>521</v>
+        <v>163</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>522</v>
+        <v>164</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>523</v>
+        <v>166</v>
       </c>
       <c r="D253" s="1" t="s">
         <v>35</v>
@@ -6537,13 +6546,13 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
-        <v>163</v>
+        <v>33</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>164</v>
+        <v>34</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>166</v>
+        <v>525</v>
       </c>
       <c r="D254" s="1" t="s">
         <v>35</v>
@@ -6551,13 +6560,13 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
-        <v>33</v>
+        <v>685</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>34</v>
+        <v>683</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>529</v>
+        <v>684</v>
       </c>
       <c r="D255" s="1" t="s">
         <v>35</v>
@@ -6565,13 +6574,13 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
-        <v>695</v>
+        <v>649</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>693</v>
+        <v>499</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>694</v>
+        <v>650</v>
       </c>
       <c r="D256" s="1" t="s">
         <v>35</v>
@@ -6579,13 +6588,13 @@
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>502</v>
+        <v>654</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="D257" s="1" t="s">
         <v>35</v>
@@ -6593,13 +6602,13 @@
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
-        <v>663</v>
+        <v>638</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>664</v>
+        <v>639</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>662</v>
+        <v>337</v>
       </c>
       <c r="D258" s="1" t="s">
         <v>35</v>
@@ -6607,117 +6616,103 @@
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
-        <v>648</v>
+        <v>540</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>649</v>
+        <v>541</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>337</v>
+        <v>542</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>35</v>
+        <v>534</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B260" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="B260" s="1" t="s">
+      <c r="C260" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="C260" s="1" t="s">
-        <v>546</v>
-      </c>
       <c r="D260" s="1" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>548</v>
+        <v>743</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>549</v>
+        <v>374</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
-        <v>555</v>
+        <v>651</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>556</v>
+        <v>744</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>376</v>
+        <v>652</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
-        <v>661</v>
+        <v>527</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>557</v>
+        <v>528</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>662</v>
+        <v>321</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>538</v>
+        <v>243</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F263" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G263" s="1" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
-        <v>531</v>
+        <v>699</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>532</v>
+        <v>696</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>321</v>
+        <v>697</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E264" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F264" s="1" t="s">
-        <v>3</v>
+        <v>698</v>
       </c>
       <c r="G264" s="1" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A265" s="1" t="s">
-        <v>709</v>
-      </c>
-      <c r="B265" s="1" t="s">
-        <v>706</v>
-      </c>
-      <c r="C265" s="1" t="s">
-        <v>707</v>
-      </c>
-      <c r="D265" s="1" t="s">
-        <v>708</v>
-      </c>
-      <c r="G265" s="1" t="s">
-        <v>723</v>
+        <v>713</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G265">
-    <sortCondition ref="D239:D265"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G264">
+    <sortCondition ref="D238:D264"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adapted for mobile devices
</commit_message>
<xml_diff>
--- a/data/lexemes.xlsx
+++ b/data/lexemes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergeimalyshev/Desktop/Tocharian/Tocharian A/My grammar/Candrakanta/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD6088E-22E1-104F-9FC4-88008A71E97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F04604D-BF2C-6E45-9B48-E5AD5EFFEE14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="760" windowWidth="25700" windowHeight="13080" xr2:uid="{DFFD3512-190B-6C44-A03E-FE8C03207A6B}"/>
+    <workbookView xWindow="720" yWindow="7220" windowWidth="25700" windowHeight="13080" xr2:uid="{DFFD3512-190B-6C44-A03E-FE8C03207A6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Affixation" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="754">
   <si>
     <t>Shape</t>
   </si>
@@ -1958,9 +1958,6 @@
     <t>Wram</t>
   </si>
   <si>
-    <t xml:space="preserve">Prār </t>
-  </si>
-  <si>
     <t>W_krase</t>
   </si>
   <si>
@@ -2271,6 +2268,36 @@
   </si>
   <si>
     <t>Morpheme_2</t>
+  </si>
+  <si>
+    <t>Prār;Kṣur</t>
+  </si>
+  <si>
+    <t>I_ynālek</t>
+  </si>
+  <si>
+    <t>elsewhere</t>
+  </si>
+  <si>
+    <t>W_wrassi</t>
+  </si>
+  <si>
+    <t>R_waro</t>
+  </si>
+  <si>
+    <t>stinky</t>
+  </si>
+  <si>
+    <t>R_warom</t>
+  </si>
+  <si>
+    <t>M_walāṃ</t>
+  </si>
+  <si>
+    <t>tent?</t>
+  </si>
+  <si>
+    <t>V_vāl</t>
   </si>
 </sst>
 </file>
@@ -2680,10 +2707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF76C2B-797E-2544-85E2-CF60CE11F59B}">
-  <dimension ref="A1:G263"/>
+  <dimension ref="A1:G268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="175" workbookViewId="0">
-      <selection activeCell="B174" sqref="B174"/>
+    <sheetView tabSelected="1" topLeftCell="A258" zoomScale="175" workbookViewId="0">
+      <selection activeCell="D268" sqref="D268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2704,13 +2731,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>743</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>744</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>578</v>
@@ -2721,7 +2748,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>71</v>
@@ -2955,13 +2982,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>729</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>730</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>731</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>67</v>
@@ -3046,7 +3073,7 @@
         <v>585</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -3074,7 +3101,7 @@
         <v>212</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>169</v>
@@ -3082,13 +3109,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>715</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>716</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>169</v>
@@ -3113,7 +3140,7 @@
         <v>590</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>108</v>
@@ -3127,7 +3154,7 @@
         <v>107</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>108</v>
@@ -3200,7 +3227,7 @@
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -3250,7 +3277,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>15</v>
@@ -3309,7 +3336,7 @@
         <v>577</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -3348,10 +3375,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>664</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>665</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>166</v>
@@ -3380,12 +3407,12 @@
         <v>577</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>12</v>
@@ -3400,16 +3427,16 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>724</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>726</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -3505,13 +3532,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>658</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>659</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>47</v>
@@ -3581,13 +3608,13 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>642</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>643</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>47</v>
@@ -3725,13 +3752,13 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>673</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>674</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>47</v>
@@ -3805,7 +3832,7 @@
         <v>47</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -3842,7 +3869,7 @@
         <v>577</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -3988,10 +4015,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>644</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>645</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>492</v>
@@ -4225,7 +4252,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>472</v>
@@ -4367,7 +4394,7 @@
         <v>577</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
@@ -4508,7 +4535,7 @@
         <v>577</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>640</v>
+        <v>744</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
@@ -4542,7 +4569,7 @@
         <v>112</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
@@ -4857,7 +4884,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>473</v>
@@ -4899,13 +4926,13 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="B140" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="C140" s="1" t="s">
         <v>670</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>671</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>59</v>
@@ -4930,7 +4957,7 @@
         <v>569</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>568</v>
@@ -4972,13 +4999,13 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="C145" s="1" t="s">
         <v>652</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>653</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>59</v>
@@ -5026,21 +5053,21 @@
         <v>59</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="D149" s="1" t="s">
         <v>655</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
@@ -5093,7 +5120,7 @@
         <v>573</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>62</v>
@@ -5229,18 +5256,18 @@
         <v>519</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="C162" s="1" t="s">
         <v>690</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>692</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>691</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>519</v>
@@ -5417,7 +5444,7 @@
         <v>25</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
@@ -5436,7 +5463,7 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>527</v>
@@ -5445,7 +5472,7 @@
         <v>6</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
@@ -5464,13 +5491,13 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="B178" s="1" t="s">
         <v>683</v>
       </c>
-      <c r="B178" s="1" t="s">
+      <c r="C178" s="1" t="s">
         <v>684</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>685</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>41</v>
@@ -5518,7 +5545,7 @@
         <v>41</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.2">
@@ -5565,10 +5592,10 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B185" s="1" t="s">
         <v>666</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>667</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>73</v>
@@ -5593,13 +5620,13 @@
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>497</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D187" s="1" t="s">
         <v>41</v>
@@ -5621,10 +5648,10 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="B189" s="1" t="s">
         <v>678</v>
-      </c>
-      <c r="B189" s="1" t="s">
-        <v>679</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>196</v>
@@ -5663,7 +5690,7 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>377</v>
@@ -5759,7 +5786,7 @@
         <v>154</v>
       </c>
       <c r="G198" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.2">
@@ -5792,10 +5819,10 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="B201" s="1" t="s">
         <v>687</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>688</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>227</v>
@@ -5806,7 +5833,7 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>497</v>
@@ -5862,13 +5889,13 @@
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="B206" s="1" t="s">
         <v>721</v>
       </c>
-      <c r="B206" s="1" t="s">
+      <c r="C206" s="1" t="s">
         <v>722</v>
-      </c>
-      <c r="C206" s="1" t="s">
-        <v>723</v>
       </c>
       <c r="D206" s="1" t="s">
         <v>154</v>
@@ -5918,13 +5945,13 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D210" s="1" t="s">
         <v>154</v>
@@ -5974,13 +6001,13 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D214" s="1" t="s">
         <v>172</v>
@@ -6002,13 +6029,13 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="B216" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="B216" s="1" t="s">
+      <c r="C216" s="1" t="s">
         <v>662</v>
-      </c>
-      <c r="C216" s="1" t="s">
-        <v>663</v>
       </c>
       <c r="D216" s="1" t="s">
         <v>172</v>
@@ -6294,7 +6321,7 @@
         <v>115</v>
       </c>
       <c r="G236" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.2">
@@ -6411,13 +6438,13 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="B245" s="1" t="s">
         <v>698</v>
       </c>
-      <c r="B245" s="1" t="s">
+      <c r="C245" s="1" t="s">
         <v>699</v>
-      </c>
-      <c r="C245" s="1" t="s">
-        <v>700</v>
       </c>
       <c r="D245" s="1" t="s">
         <v>35</v>
@@ -6537,13 +6564,13 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B254" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="C254" s="1" t="s">
         <v>680</v>
-      </c>
-      <c r="C254" s="1" t="s">
-        <v>681</v>
       </c>
       <c r="D254" s="1" t="s">
         <v>35</v>
@@ -6551,13 +6578,13 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>497</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D255" s="1" t="s">
         <v>35</v>
@@ -6565,13 +6592,13 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="B256" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="B256" s="1" t="s">
-        <v>651</v>
-      </c>
       <c r="C256" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D256" s="1" t="s">
         <v>35</v>
@@ -6624,7 +6651,7 @@
         <v>548</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>372</v>
@@ -6635,13 +6662,13 @@
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="C261" s="1" t="s">
         <v>648</v>
-      </c>
-      <c r="B261" s="1" t="s">
-        <v>741</v>
-      </c>
-      <c r="C261" s="1" t="s">
-        <v>649</v>
       </c>
       <c r="D261" s="1" t="s">
         <v>532</v>
@@ -6672,19 +6699,89 @@
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B263" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="C263" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="C263" s="1" t="s">
+      <c r="D263" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="D263" s="1" t="s">
-        <v>695</v>
-      </c>
       <c r="G263" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A264" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D264" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A265" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A266" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A267" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A268" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="D268" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the show all variants button for verbs
</commit_message>
<xml_diff>
--- a/data/lexemes.xlsx
+++ b/data/lexemes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergeimalyshev/Desktop/Tocharian/Tocharian A/My grammar/Candrakanta/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F04604D-BF2C-6E45-9B48-E5AD5EFFEE14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8424CA6-B732-CD42-B239-671D48B44F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="7220" windowWidth="25700" windowHeight="13080" xr2:uid="{DFFD3512-190B-6C44-A03E-FE8C03207A6B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="754">
   <si>
     <t>Shape</t>
   </si>
@@ -2709,8 +2709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF76C2B-797E-2544-85E2-CF60CE11F59B}">
   <dimension ref="A1:G268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" zoomScale="175" workbookViewId="0">
-      <selection activeCell="D268" sqref="D268"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="175" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3041,6 +3041,9 @@
       <c r="D20" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="G20" s="1" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">

</xml_diff>

<commit_message>
Less optional homonymous variants get precedence
</commit_message>
<xml_diff>
--- a/data/lexemes.xlsx
+++ b/data/lexemes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergeimalyshev/Desktop/Tocharian/Tocharian A/My grammar/Candrakanta/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805CBB58-E53D-6445-9E57-FBBF2CFBAF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DDBF00-5B8D-164E-87E4-496589B68B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3740" yWindow="2500" windowWidth="25700" windowHeight="14000" xr2:uid="{DFFD3512-190B-6C44-A03E-FE8C03207A6B}"/>
   </bookViews>
@@ -2758,7 +2758,7 @@
   <dimension ref="A1:G275"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>